<commit_message>
Changes to add approval path
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -3,18 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aseem\eclipse-workspace\GapTestAutomation\src\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20172" windowHeight="10968" xr2:uid="{2DC61233-0395-417A-8BE6-2A6AAB79EEE7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27912" windowHeight="10968" activeTab="1" xr2:uid="{2DC61233-0395-417A-8BE6-2A6AAB79EEE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:R36"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
   <si>
     <t>Ink-Jet Printers</t>
   </si>
@@ -51,6 +48,9 @@
   </si>
   <si>
     <t>OD SAQQARA</t>
+  </si>
+  <si>
+    <t>Laser Printers</t>
   </si>
 </sst>
 </file>
@@ -404,8 +404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5141C4A7-131B-4316-A028-46944CF06F33}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -417,7 +417,7 @@
     <col min="13" max="13" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -514,6 +514,71 @@
         <v>6</v>
       </c>
       <c r="P2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCB2794B-E549-4527-84C4-D4936E8302B1}">
+  <dimension ref="A1:P1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>500</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>100</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K1" t="b">
+        <v>0</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
after merging from master
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27912" windowHeight="10968" activeTab="1" xr2:uid="{2DC61233-0395-417A-8BE6-2A6AAB79EEE7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22152" windowHeight="7716" xr2:uid="{2DC61233-0395-417A-8BE6-2A6AAB79EEE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:R36"/>
+  <oleSize ref="A1:P25"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -404,7 +404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5141C4A7-131B-4316-A028-46944CF06F33}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -526,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCB2794B-E549-4527-84C4-D4936E8302B1}">
   <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>